<commit_message>
Finalizei aula 5 e o módulo 1 de Excel
</commit_message>
<xml_diff>
--- a/Excel VBA/Aula 5 - Imprimir e Compartilhar/Produtos.xlsx
+++ b/Excel VBA/Aula 5 - Imprimir e Compartilhar/Produtos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 4 - Criando Gráficos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 5 - Imprimir e Compartilhar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0A005-D987-4BB5-8A66-9AD62E3EE416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC11CE6-FD42-44E4-B124-FF438C7E014D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{F429CDF2-33A2-4A6E-9034-27FA88637C5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{F429CDF2-33A2-4A6E-9034-27FA88637C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos Adultos" sheetId="3" r:id="rId1"/>
@@ -3059,9 +3059,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6CF0F7-701F-4AD3-A160-66200CB65652}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" activeCellId="1" sqref="A2:A11 E2:E11"/>
     </sheetView>
   </sheetViews>
@@ -3343,21 +3346,26 @@
     <mergeCell ref="C13:F13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DC4B28-A0EC-435B-9AD3-BBF63385D2CE}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="91" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>